<commit_message>
Module 1 to 2.1 bug free
-Create, reborder and delete rows of financial assets on update sheet
-rebordering already rebordered cells causes error
</commit_message>
<xml_diff>
--- a/exe/Utilities.xlsx
+++ b/exe/Utilities.xlsx
@@ -375,7 +375,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -383,7 +383,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -391,7 +391,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -399,7 +399,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>